<commit_message>
updating base library namespace
</commit_message>
<xml_diff>
--- a/resources/SchoolMngr Model.xlsx
+++ b/resources/SchoolMngr Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\-Projects\SchoolMngr.MSvc\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\SchoolMngrMSvc\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>Grade</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Backoffice</t>
   </si>
   <si>
-    <t>MaxAbsencesAllowed</t>
-  </si>
-  <si>
     <t>MinExamScoreRequired</t>
   </si>
   <si>
@@ -216,6 +213,12 @@
   </si>
   <si>
     <t>AcadStateFK</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>MinAttendanceRequired</t>
   </si>
 </sst>
 </file>
@@ -597,13 +600,13 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -622,7 +625,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="H2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -771,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -792,7 +795,7 @@
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="L6" t="s">
         <v>20</v>
@@ -833,7 +836,7 @@
         <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
         <v>24</v>
@@ -865,10 +868,10 @@
         <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M8" t="s">
         <v>20</v>
@@ -879,7 +882,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -891,7 +894,7 @@
         <v>48</v>
       </c>
       <c r="K9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O9" t="s">
         <v>55</v>
@@ -899,13 +902,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="O10" t="s">
         <v>57</v>
@@ -914,6 +917,9 @@
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>46</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
       </c>
       <c r="O11" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
replacing ocelot for envoy gateway
</commit_message>
<xml_diff>
--- a/resources/SchoolMngr Model.xlsx
+++ b/resources/SchoolMngr Model.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Develop\SchoolMngrMSvc\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3620573-C743-4F50-B14D-28C165F54D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5910"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Grade</t>
   </si>
@@ -219,12 +220,15 @@
   </si>
   <si>
     <t>MinAttendanceRequired</t>
+  </si>
+  <si>
+    <t>ProfileId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -596,14 +600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -792,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
         <v>12</v>
@@ -833,7 +837,7 @@
         <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
         <v>45</v>
@@ -865,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K8" t="s">
         <v>43</v>
@@ -890,11 +894,11 @@
       <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="J9" t="s">
-        <v>48</v>
-      </c>
       <c r="K9" t="s">
         <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>65</v>
       </c>
       <c r="O9" t="s">
         <v>55</v>

</xml_diff>